<commit_message>
Processreport ready for review
</commit_message>
<xml_diff>
--- a/Resources/Documents/CitizenTaxi.xlsx
+++ b/Resources/Documents/CitizenTaxi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Documents\Github\Techcollege\Education\Module 6\CitizenTaxi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Documents\Github\Techcollege\Education\Module 6\CitizenTaxi\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A038860-B276-4624-8F4E-48D83FBB2A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719048B1-6A1E-417B-A857-603D72AC980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45120" yWindow="-4995" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
+    <workbookView xWindow="-28920" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravsspec" sheetId="3" r:id="rId1"/>
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EB829-7EF3-4323-B00C-E54D52F1FFB2}">
   <dimension ref="B1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,7 +2361,7 @@
       <c r="U7" s="41"/>
       <c r="V7" s="41"/>
       <c r="W7" s="41"/>
-      <c r="X7" s="40"/>
+      <c r="X7" s="41"/>
       <c r="Y7" s="42"/>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
@@ -2391,7 +2391,7 @@
       <c r="U8" s="41"/>
       <c r="V8" s="41"/>
       <c r="W8" s="41"/>
-      <c r="X8" s="20"/>
+      <c r="X8" s="41"/>
       <c r="Y8" s="24"/>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
       <c r="U13" s="18"/>
       <c r="V13" s="22"/>
       <c r="W13" s="22"/>
-      <c r="X13" s="22"/>
+      <c r="X13" s="18"/>
       <c r="Y13" s="26"/>
     </row>
     <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>